<commit_message>
Output files with model answers from evaluation function in chat.py
</commit_message>
<xml_diff>
--- a/Forkin-Finding-llama3.2.xlsx
+++ b/Forkin-Finding-llama3.2.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+  <si>
+    <t>DOCUMENT</t>
+  </si>
   <si>
     <t>QUESTION</t>
   </si>
@@ -22,7 +25,10 @@
     <t>CORRECT_ANSWER</t>
   </si>
   <si>
-    <t>MODEL_ANSWER</t>
+    <t>LLM_ANSWER</t>
+  </si>
+  <si>
+    <t>forkin-finding-llama3.2</t>
   </si>
   <si>
     <t>Who was the deceased?</t>
@@ -91,17 +97,10 @@
     <t>The coroner found that Luke Forkin committed suicide by hanging while absent without leave from Graylands Hospital. The care, treatment, and supervision were reasonable and appropriate, and the decision to grant unescorted ground access was justified by his apparent stability (pages 20–21).</t>
   </si>
   <si>
-    <t>Based on the provided context information, the deceased was a person who:
-- Was born in Western Australia in 1982
-- Had a blended family background with three relationships between his mother's partners
-- Experienced a close relationship with his mother and step-father when he was young
-- Had trouble fitting in at school and became a loner as he grew older
-- Developed a history of substance abuse, including amphetamines, cannabis, heroin, LSD, ecstasy, and possibly alcohol
-- Suffered a gunshot wound to the abdomen at the age of 20 due to an accident involving his step-father
-However, without any additional information or context, it is not possible to determine the deceased's specific identity or personal details beyond what is provided in the context information.</t>
-  </si>
-  <si>
-    <t>Based on the context information provided, the date of the death is unknown without additional details. However, it can be inferred that the death occurred sometime between 7.00pm on November 29th, 2010 (when the deceased arrived at Nathan Ward's house) and 12.00am or 1.00am on November 30th, 2010 (when Mr. Ward saw the deceased walking back to his bedroom).</t>
+    <t>The deceased was a man who was born in Western Australia on 23 October 1982. Unfortunately, he died from gunshot wounds to his abdomen received during an accident involving his stepfather with a handgun, resulting in significant injuries including losing part of his pancreas and kidney and fracturing two vertebrae.</t>
+  </si>
+  <si>
+    <t>The exact date of the death is not explicitly stated in the provided text. However, based on the events leading up to the death, it can be inferred that the death occurred sometime after 7:00 pm on November 29, 2010, when the deceased was seen walking back to his bedroom by Mr Ward at around 12:00 am or 1:00 am.</t>
   </si>
   <si>
     <t>The death occurred at 33A Snowbird Gardens, Joondalup.</t>
@@ -110,43 +109,40 @@
     <t>The cause of death was ligature compression of the neck (hanging).</t>
   </si>
   <si>
-    <t>The Coroner mentioned in the context is Ms R Hartley. However, it's also stated that there is a counselor appearing on behalf of her, which is Ms M. Smith assisting the Coroner. It does not explicitly state that Ms Hartley was the presiding coroner but rather mentions that she is a Coroner and Ms Smith is assisting her.</t>
-  </si>
-  <si>
-    <t>The circumstances leading to the death were as follows:
-- Mr. Ward and his wife left for work at 6:30 am, assuming the deceased was still asleep in bed.
-- They returned home from work around 4:00 pm and found the front door locked, with the deceased hanging by his neck from an electrical cord tied to a rafter through an open manhole in the ceiling.
-- Mr. Ward cut the electrical cord and applied chest compressions until ambulance paramedics arrived.
-- Upon arrival of the paramedics, they found that the deceased showed no signs of life.
-These events led to the discovery of the deceased's body and ultimately resulted in his death by asphyxiation due to neck compression, with the manner of death being suicide.</t>
-  </si>
-  <si>
-    <t>Based on the provided context information, the deceased had a history of:
-* Suicidal self-harm (2005)
-* Auditory hallucinations (2005)
-* Psychotic symptoms of schizophrenia (discharged in 2005)
-* Drug withdrawal (discharged in 2005)
-* Amphetamine-induced psychosis (diagnosed in 2006, after using amphetamines)
-* Ongoing paranoid psychotic episodes exacerbated by substance abuse (2006)
-* Suicidal behavior (2007), including attempting to kill himself with petrol
-* Resumed intravenous amphetamine use (leading up to his 2007 hospitalization)
-Additionally, he had experienced relationship issues and housing difficulties in the lead-up to his 2007 hospitalization.</t>
-  </si>
-  <si>
-    <t>Based on the provided context information, it can be inferred that the following individuals assisted or testified in the inquest:
-1. Coroner DH Mulligan
-2. Evelyn Vicker (Acting State Coroner)
-3. Interested parties who were present at the inquests before Coroner Mulligan, but their specific roles are not mentioned.
-No other individuals are specifically mentioned as assisting or testifying in the inquest.</t>
-  </si>
-  <si>
-    <t>Yes, based on the context information provided, it appears that Luke Isaac Forkin was considered a "person held in care" under the Coroners Act 1996. This is explicitly stated in section 3 of the Coroners Act 1996, which defines who falls within this category. As an involuntary patient at Graylands Hospital, he met the criteria to be considered a "person held in care".</t>
-  </si>
-  <si>
-    <t>Yes, there was evidence of substances found in the deceased's body. The toxicology analysis showed therapeutic and sub-therapeutic levels of prescription medicines, as well as a low level of tetrahydrocannabinol (THC), indicating use of cannabis within 24 hours prior to death.</t>
-  </si>
-  <si>
-    <t>Based on the provided context, it appears that the coroner did not comment extensively on general systemic issues related to Graylands Hospital, as they were not deemed sufficiently connected to all of the respective deaths. However, some general evidence was considered to provide an overview of the context in which the deceased persons were treated for their mental illnesses.</t>
+    <t>Based on the provided context, Ms R Hartley was the Coroner.</t>
+  </si>
+  <si>
+    <t>The deceased was found hanging from an electrical cord tied to a rafter through an open manhole in the ceiling of his home. Mr. Ward discovered him at around 4:00pm on the next morning after returning home from work, and called emergency services. The ambulance paramedics arrived shortly after but were unable to revive him.</t>
+  </si>
+  <si>
+    <t>The deceased had a significant history of mental health issues and substance abuse. The following are some relevant aspects of his medical and mental health history:
+1. Schizophrenia: Diagnosed with psychotic symptoms of schizophrenia in 2005.
+2. Amphetamine-induced psychosis: Experienced two episodes of psychosis secondary to amphetamine use, one in 2005 and another in June 2006.
+3. Suicidal behavior: Exhibited suicidal ideation on multiple occasions, including in 2005 and November 2007.
+4. Auditory hallucinations: Experienced auditory hallucinations in 2005.
+5. Substance abuse: Engaged in intravenous amphetamine use, which led to psychosis and other mental health issues.
+6. Depression or relationship-related stress: Experiencing relationship difficulties with a partner, leading to suicidal behavior and housing instability.
+7. Treatment: Received treatment with olanzapine at Graylands Hospital.
+Overall, the deceased's history suggests that he struggled with severe mental health issues, including schizophrenia and amphetamine-induced psychosis, which were exacerbated by substance abuse and life stressors.</t>
+  </si>
+  <si>
+    <t>Based on the provided context, the following individuals are mentioned as having assisted or testified in the inquest:
+1. Coroner DH. Mulligan
+2. Acting State Coroner Evelyn Vicker
+It is also implied that other interested parties who were present at the inquests before Coroner Mulligan made submissions during the subsequent inquest held by the author (the person making this answer).</t>
+  </si>
+  <si>
+    <t>Yes, based on the given context information, the deceased (Luke Isaac Forkin) was considered a "person held in care" under the Coroners Act 1996. According to section 3 of the Coroners Act 1996, as he was an involuntary patient at Graylands Hospital at the time of his death.</t>
+  </si>
+  <si>
+    <t>Yes, there was evidence of substances found in the deceased's body. The toxicology analysis showed:
+* Therapeutic levels of prescription medicines
+* Sub-therapeutic levels of prescription medicines (not specified which)
+* A low level of tetrahydrocannabinol (THC), indicating use of cannabis within 24 hours.
+No specific details about amphetamines were mentioned, apart from stating he began using them at age 14.</t>
+  </si>
+  <si>
+    <t>Based on the provided context, the coroner did not address general issues separately from their individual death findings. Instead, they considered general or systemic issues related to Graylands (a mental health facility) that were relevant to the quality of supervision, treatment, and care of the deceased patients, but only commented on these issues in a limited capacity under section 25 due to insufficient connection with all the respective deaths.</t>
   </si>
 </sst>
 </file>
@@ -504,13 +500,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,126 +516,162 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
+      <c r="D12" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>